<commit_message>
DDR3 control and address lines tunned to match the clock by 10ps. Banks 1 and 0 will follow.
</commit_message>
<xml_diff>
--- a/DDR3 board timings.xlsx
+++ b/DDR3 board timings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CERN\APD\IPMC\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CERN\APD\IPMC\Schematic\svn\trunk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1162,17 +1162,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="99">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1340,816 +1330,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3702,8 +2882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3766,7 +2946,7 @@
         <v>171</v>
       </c>
       <c r="Q1" s="10">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="R1" s="6" t="s">
         <v>173</v>
@@ -3787,7 +2967,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D2">
-        <v>647.23199999999997</v>
+        <v>772.19399999999996</v>
       </c>
       <c r="F2">
         <v>24.315000000000001</v>
@@ -3797,7 +2977,7 @@
       </c>
       <c r="J2" s="5">
         <f>B2+(C2+H2)/1000*io_1!$J$1+(D2+F2*2+G2*2)/1000*io_1!$J$2</f>
-        <v>183.91017457999999</v>
+        <v>204.52178174599999</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="9" t="s">
@@ -3811,7 +2991,7 @@
         <v>172</v>
       </c>
       <c r="Q2">
-        <v>103</v>
+        <v>10</v>
       </c>
       <c r="R2" s="6" t="s">
         <v>173</v>
@@ -3832,7 +3012,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D3">
-        <v>665.05399999999997</v>
+        <v>788.33699999999999</v>
       </c>
       <c r="F3">
         <v>24.315000000000001</v>
@@ -3842,7 +3022,7 @@
       </c>
       <c r="J3" s="5">
         <f>B3+(C3+H3)/1000*io_1!$J$1+(D3+F3*2+G3*2)/1000*io_1!$J$2</f>
-        <v>183.95928872600001</v>
+        <v>204.29395659500003</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -3856,14 +3036,14 @@
       </c>
       <c r="C4" s="11">
         <f>MAX(J2:J3)-MIN(J2:J3)</f>
-        <v>4.9114146000022174E-2</v>
+        <v>0.22782515099996203</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>179</v>
       </c>
       <c r="J4" s="9">
         <f>AVERAGE(J2:J3)</f>
-        <v>183.934731653</v>
+        <v>204.40786917050002</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -3871,7 +3051,7 @@
         <v>184</v>
       </c>
       <c r="Q4">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -3965,11 +3145,11 @@
       </c>
       <c r="K8" s="5">
         <f>$J$4-J8</f>
-        <v>-24.609115628999973</v>
+        <v>-4.1359781114999521</v>
       </c>
       <c r="L8" s="5">
         <f>K8/io_1!$J$2*1000</f>
-        <v>-149.19769634964788</v>
+        <v>-25.075196349647765</v>
       </c>
       <c r="M8" t="str">
         <f>IF(J8=$R$8, "Route","")</f>
@@ -3980,7 +3160,7 @@
       </c>
       <c r="O8" s="5">
         <f>MIN(J8:J30)</f>
-        <v>135.98643510799999</v>
+        <v>197.10024950500002</v>
       </c>
       <c r="Q8">
         <f>IF(D8=0,J8,0)</f>
@@ -3996,7 +3176,7 @@
       </c>
       <c r="T8">
         <f>MIN(S8:S30)</f>
-        <v>135.98643510799999</v>
+        <v>197.10024950500002</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -4011,7 +3191,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D9">
-        <v>547.17700000000002</v>
+        <v>828.26700000000005</v>
       </c>
       <c r="F9">
         <v>12.635</v>
@@ -4021,15 +3201,15 @@
       </c>
       <c r="J9" s="5">
         <f>B9+(C9+H9+E9)/1000*io_1!$J$1+(D9+F9*2+G9*2)/1000*io_1!$J$2</f>
-        <v>152.284734235</v>
+        <v>198.64856210500002</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" ref="K9:K30" si="0">$J$4-J9</f>
-        <v>31.649997417999998</v>
+        <v>5.7593070654999963</v>
       </c>
       <c r="L9" s="5">
         <f>K9/io_1!$J$2*1000</f>
-        <v>191.88445352636967</v>
+        <v>34.916953526369689</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" ref="M9:M30" si="1">IF(J9=$R$8, "Route","")</f>
@@ -4048,7 +3228,7 @@
       </c>
       <c r="S9">
         <f t="shared" ref="S9:S30" si="3">IF(D9=0,"",J9)</f>
-        <v>152.284734235</v>
+        <v>198.64856210500002</v>
       </c>
       <c r="T9">
         <f>MAX(S8:S30)</f>
@@ -4067,7 +3247,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D10">
-        <v>560.22199999999998</v>
+        <v>895.70699999999999</v>
       </c>
       <c r="F10">
         <v>12.635</v>
@@ -4077,15 +3257,15 @@
       </c>
       <c r="J10" s="5">
         <f>B10+(C10+H10+E10)/1000*io_1!$J$1+(D10+F10*2+G10*2)/1000*io_1!$J$2</f>
-        <v>155.34291567</v>
+        <v>210.678818025</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="0"/>
-        <v>28.591815983000004</v>
+        <v>-6.2709488544999772</v>
       </c>
       <c r="L10" s="5">
         <f>K10/io_1!$J$2*1000</f>
-        <v>173.34361557022729</v>
+        <v>-38.018884429772569</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
@@ -4097,7 +3277,7 @@
       </c>
       <c r="S10">
         <f t="shared" si="3"/>
-        <v>155.34291567</v>
+        <v>210.678818025</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -4112,7 +3292,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D11">
-        <v>539.53399999999999</v>
+        <v>888.46100000000001</v>
       </c>
       <c r="F11">
         <v>9.0549999999999997</v>
@@ -4122,15 +3302,15 @@
       </c>
       <c r="J11" s="5">
         <f>B11+(C11+H11+E11)/1000*io_1!$J$1+(D11+F11*2+G11*2)/1000*io_1!$J$2</f>
-        <v>142.422583006</v>
+        <v>199.97564916700003</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="0"/>
-        <v>41.512148647000004</v>
+        <v>4.4322200034999923</v>
       </c>
       <c r="L11" s="5">
         <f>K11/io_1!$J$2*1000</f>
-        <v>251.67572220100277</v>
+        <v>26.871222201002723</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="1"/>
@@ -4142,7 +3322,7 @@
       </c>
       <c r="S11">
         <f t="shared" si="3"/>
-        <v>142.422583006</v>
+        <v>199.97564916700003</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
@@ -4160,7 +3340,7 @@
         <v>541.84</v>
       </c>
       <c r="E12">
-        <v>188.976</v>
+        <v>301.12299999999999</v>
       </c>
       <c r="F12">
         <v>9.0549999999999997</v>
@@ -4173,15 +3353,15 @@
       </c>
       <c r="J12" s="5">
         <f>B12+(C12+H12+E12)/1000*io_1!$J$1+(D12+F12*2+G12*2)/1000*io_1!$J$2</f>
-        <v>183.64896388599999</v>
+        <v>200.27666313500001</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="0"/>
-        <v>0.28576776700001005</v>
+        <v>4.1312060355000142</v>
       </c>
       <c r="L12" s="5">
         <f>K12/io_1!$J$2*1000</f>
-        <v>1.7325243690245118</v>
+        <v>25.046264682344894</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="1"/>
@@ -4193,7 +3373,7 @@
       </c>
       <c r="S12">
         <f t="shared" si="3"/>
-        <v>183.64896388599999</v>
+        <v>200.27666313500001</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -4208,7 +3388,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D13">
-        <v>570.17100000000005</v>
+        <v>868.75599999999997</v>
       </c>
       <c r="F13">
         <v>12.635</v>
@@ -4218,15 +3398,15 @@
       </c>
       <c r="J13" s="5">
         <f>B13+(C13+H13+E13)/1000*io_1!$J$1+(D13+F13*2+G13*2)/1000*io_1!$J$2</f>
-        <v>155.35543357700001</v>
+        <v>204.60493923200002</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="0"/>
-        <v>28.579298075999986</v>
+        <v>-0.19707006149999984</v>
       </c>
       <c r="L13" s="5">
         <f>K13/io_1!$J$2*1000</f>
-        <v>173.26772324984984</v>
+        <v>-1.1947767501500508</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="1"/>
@@ -4238,7 +3418,7 @@
       </c>
       <c r="S13">
         <f t="shared" si="3"/>
-        <v>155.35543357700001</v>
+        <v>204.60493923200002</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
@@ -4267,11 +3447,11 @@
       </c>
       <c r="K14" s="5">
         <f t="shared" si="0"/>
-        <v>-15.111895150000009</v>
+        <v>5.3612423675000116</v>
       </c>
       <c r="L14" s="5">
         <f>K14/io_1!$J$2*1000</f>
-        <v>-91.618893496541276</v>
+        <v>32.50360650345884</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="1"/>
@@ -4298,7 +3478,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D15">
-        <v>452.68799999999999</v>
+        <v>860.48599999999999</v>
       </c>
       <c r="F15">
         <v>12.635</v>
@@ -4308,15 +3488,15 @@
       </c>
       <c r="J15" s="5">
         <f>B15+(C15+H15+E15)/1000*io_1!$J$1+(D15+F15*2+G15*2)/1000*io_1!$J$2</f>
-        <v>135.98643510799999</v>
+        <v>203.249860622</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="0"/>
-        <v>47.948296545000005</v>
+        <v>1.1580085485000211</v>
       </c>
       <c r="L15" s="5">
         <f>K15/io_1!$J$2*1000</f>
-        <v>290.69615894581761</v>
+        <v>7.0206589458177735</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="1"/>
@@ -4328,7 +3508,7 @@
       </c>
       <c r="S15">
         <f t="shared" si="3"/>
-        <v>135.98643510799999</v>
+        <v>203.249860622</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
@@ -4343,7 +3523,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D16">
-        <v>491.89400000000001</v>
+        <v>809.16099999999994</v>
       </c>
       <c r="F16">
         <v>27.895</v>
@@ -4353,15 +3533,15 @@
       </c>
       <c r="J16" s="5">
         <f>B16+(C16+H16+E16)/1000*io_1!$J$1+(D16+F16*2+G16*2)/1000*io_1!$J$2</f>
-        <v>145.371250726</v>
+        <v>197.70222150699999</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="0"/>
-        <v>38.563480927000001</v>
+        <v>6.7056476635000308</v>
       </c>
       <c r="L16" s="5">
         <f>K16/io_1!$J$2*1000</f>
-        <v>233.79883309385664</v>
+        <v>40.654333093856849</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="1"/>
@@ -4373,7 +3553,7 @@
       </c>
       <c r="S16">
         <f t="shared" si="3"/>
-        <v>145.371250726</v>
+        <v>197.70222150699999</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -4388,10 +3568,10 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D17">
-        <v>397.40600000000001</v>
+        <v>365.91</v>
       </c>
       <c r="E17">
-        <v>94.388000000000005</v>
+        <v>447.46800000000002</v>
       </c>
       <c r="F17">
         <v>9.0549999999999997</v>
@@ -4404,15 +3584,15 @@
       </c>
       <c r="J17" s="5">
         <f>B17+(C17+H17+E17)/1000*io_1!$J$1+(D17+F17*2+G17*2)/1000*io_1!$J$2</f>
-        <v>151.28830762799998</v>
+        <v>198.44337526000001</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="0"/>
-        <v>32.646424025000016</v>
+        <v>5.9644939105000105</v>
       </c>
       <c r="L17" s="5">
         <f>K17/io_1!$J$2*1000</f>
-        <v>197.92548956306126</v>
+        <v>36.160939903481868</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="1"/>
@@ -4424,7 +3604,7 @@
       </c>
       <c r="S17">
         <f t="shared" si="3"/>
-        <v>151.28830762799998</v>
+        <v>198.44337526000001</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
@@ -4439,7 +3619,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D18">
-        <v>807.64599999999996</v>
+        <v>883.68399999999997</v>
       </c>
       <c r="F18">
         <v>27.895</v>
@@ -4449,15 +3629,15 @@
       </c>
       <c r="J18" s="5">
         <f>B18+(C18+H18+E18)/1000*io_1!$J$1+(D18+F18*2+G18*2)/1000*io_1!$J$2</f>
-        <v>192.13533286199998</v>
+        <v>204.677268696</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="0"/>
-        <v>-8.2006012089999842</v>
+        <v>-0.2693995254999777</v>
       </c>
       <c r="L18" s="5">
         <f>K18/io_1!$J$2*1000</f>
-        <v>-49.717788623948778</v>
+        <v>-1.6332886239487439</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="1"/>
@@ -4469,7 +3649,7 @@
       </c>
       <c r="S18">
         <f t="shared" si="3"/>
-        <v>192.13533286199998</v>
+        <v>204.677268696</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
@@ -4484,7 +3664,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D19">
-        <v>660.27800000000002</v>
+        <v>879.16800000000001</v>
       </c>
       <c r="F19">
         <v>12.635</v>
@@ -4494,15 +3674,15 @@
       </c>
       <c r="J19" s="5">
         <f>B19+(C19+H19+E19)/1000*io_1!$J$1+(D19+F19*2+G19*2)/1000*io_1!$J$2</f>
-        <v>161.95295247800001</v>
+        <v>198.05732574799998</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="0"/>
-        <v>21.981779174999986</v>
+        <v>6.3505434225000386</v>
       </c>
       <c r="L19" s="5">
         <f>K19/io_1!$J$2*1000</f>
-        <v>133.26894245284726</v>
+        <v>38.501442452847577</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="1"/>
@@ -4514,7 +3694,7 @@
       </c>
       <c r="S19">
         <f t="shared" si="3"/>
-        <v>161.95295247800001</v>
+        <v>198.05732574799998</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
@@ -4529,7 +3709,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D20">
-        <v>732.72699999999998</v>
+        <v>870.803</v>
       </c>
       <c r="F20">
         <v>27.895</v>
@@ -4539,15 +3719,15 @@
       </c>
       <c r="J20" s="5">
         <f>B20+(C20+H20+E20)/1000*io_1!$J$1+(D20+F20*2+G20*2)/1000*io_1!$J$2</f>
-        <v>183.79496824499998</v>
+        <v>206.56963791300001</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="0"/>
-        <v>0.13976340800002163</v>
+        <v>-2.1617687424999872</v>
       </c>
       <c r="L20" s="5">
         <f>K20/io_1!$J$2*1000</f>
-        <v>0.84734367630042873</v>
+        <v>-13.106156323699624</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="1"/>
@@ -4559,7 +3739,7 @@
       </c>
       <c r="S20">
         <f t="shared" si="3"/>
-        <v>183.79496824499998</v>
+        <v>206.56963791300001</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
@@ -4574,7 +3754,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D21">
-        <v>544.07899999999995</v>
+        <v>869.71100000000001</v>
       </c>
       <c r="F21">
         <v>12.635</v>
@@ -4584,15 +3764,15 @@
       </c>
       <c r="J21" s="5">
         <f>B21+(C21+H21+E21)/1000*io_1!$J$1+(D21+F21*2+G21*2)/1000*io_1!$J$2</f>
-        <v>145.19874082099997</v>
+        <v>198.90945979700001</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="0"/>
-        <v>38.735990832000027</v>
+        <v>5.4984093735000101</v>
       </c>
       <c r="L21" s="5">
         <f>K21/io_1!$J$2*1000</f>
-        <v>234.84470897219055</v>
+        <v>33.335208972190451</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="1"/>
@@ -4604,7 +3784,7 @@
       </c>
       <c r="S21">
         <f t="shared" si="3"/>
-        <v>145.19874082099997</v>
+        <v>198.90945979700001</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
@@ -4619,7 +3799,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D22">
-        <v>617.87900000000002</v>
+        <v>809.48900000000003</v>
       </c>
       <c r="F22">
         <v>27.895</v>
@@ -4629,15 +3809,15 @@
       </c>
       <c r="J22" s="5">
         <f>B22+(C22+H22+E22)/1000*io_1!$J$1+(D22+F22*2+G22*2)/1000*io_1!$J$2</f>
-        <v>168.91209458099999</v>
+        <v>200.51682281100003</v>
       </c>
       <c r="K22" s="5">
         <f t="shared" si="0"/>
-        <v>15.022637072000009</v>
+        <v>3.8910463594999953</v>
       </c>
       <c r="L22" s="5">
         <f>K22/io_1!$J$2*1000</f>
-        <v>91.077748507060065</v>
+        <v>23.590248507059986</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="1"/>
@@ -4649,7 +3829,7 @@
       </c>
       <c r="S22">
         <f t="shared" si="3"/>
-        <v>168.91209458099999</v>
+        <v>200.51682281100003</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
@@ -4664,7 +3844,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D23">
-        <v>415.85599999999999</v>
+        <v>774.00800000000004</v>
       </c>
       <c r="F23">
         <v>9.0549999999999997</v>
@@ -4674,15 +3854,15 @@
       </c>
       <c r="J23" s="5">
         <f>B23+(C23+H23+E23)/1000*io_1!$J$1+(D23+F23*2+G23*2)/1000*io_1!$J$2</f>
-        <v>138.93926265200002</v>
+        <v>198.01392798800003</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="0"/>
-        <v>44.995469000999975</v>
+        <v>6.3939411824999866</v>
       </c>
       <c r="L23" s="5">
         <f>K23/io_1!$J$2*1000</f>
-        <v>272.79405007184283</v>
+        <v>38.764550071842912</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="1"/>
@@ -4694,7 +3874,7 @@
       </c>
       <c r="S23">
         <f t="shared" si="3"/>
-        <v>138.93926265200002</v>
+        <v>198.01392798800003</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
@@ -4709,7 +3889,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D24">
-        <v>617.87800000000004</v>
+        <v>841.94</v>
       </c>
       <c r="F24">
         <v>27.895</v>
@@ -4719,15 +3899,15 @@
       </c>
       <c r="J24" s="5">
         <f>B24+(C24+H24+E24)/1000*io_1!$J$1+(D24+F24*2+G24*2)/1000*io_1!$J$2</f>
-        <v>167.03542963800001</v>
+        <v>203.992888104</v>
       </c>
       <c r="K24" s="5">
         <f t="shared" si="0"/>
-        <v>16.899302014999989</v>
+        <v>0.41498106650001887</v>
       </c>
       <c r="L24" s="5">
         <f>K24/io_1!$J$2*1000</f>
-        <v>102.45540589779492</v>
+        <v>2.5159058977951103</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="1"/>
@@ -4739,7 +3919,7 @@
       </c>
       <c r="S24">
         <f t="shared" si="3"/>
-        <v>167.03542963800001</v>
+        <v>203.992888104</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
@@ -4754,7 +3934,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D25">
-        <v>697.01400000000001</v>
+        <v>809.16099999999994</v>
       </c>
       <c r="F25">
         <v>9.0549999999999997</v>
@@ -4764,15 +3944,15 @@
       </c>
       <c r="J25" s="5">
         <f>B25+(C25+H25+E25)/1000*io_1!$J$1+(D25+F25*2+G25*2)/1000*io_1!$J$2</f>
-        <v>189.47530664600001</v>
+        <v>207.973169267</v>
       </c>
       <c r="K25" s="5">
         <f t="shared" si="0"/>
-        <v>-5.540574993000007</v>
+        <v>-3.5653000964999819</v>
       </c>
       <c r="L25" s="5">
         <f>K25/io_1!$J$2*1000</f>
-        <v>-33.590846492424696</v>
+        <v>-21.615346492424546</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="1"/>
@@ -4784,7 +3964,7 @@
       </c>
       <c r="S25">
         <f t="shared" si="3"/>
-        <v>189.47530664600001</v>
+        <v>207.973169267</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
@@ -4799,7 +3979,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D26">
-        <v>463.66</v>
+        <v>606.90700000000004</v>
       </c>
       <c r="F26">
         <v>9.0549999999999997</v>
@@ -4809,15 +3989,15 @@
       </c>
       <c r="J26" s="5">
         <f>B26+(C26+H26+E26)/1000*io_1!$J$1+(D26+F26*2+G26*2)/1000*io_1!$J$2</f>
-        <v>173.47265958400001</v>
+        <v>197.10024950500002</v>
       </c>
       <c r="K26" s="5">
         <f t="shared" si="0"/>
-        <v>10.462072068999987</v>
+        <v>7.307619665499999</v>
       </c>
       <c r="L26" s="5">
         <f>K26/io_1!$J$2*1000</f>
-        <v>63.428409020085645</v>
+        <v>44.303909020085719</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="1"/>
@@ -4829,7 +4009,7 @@
       </c>
       <c r="S26">
         <f t="shared" si="3"/>
-        <v>173.47265958400001</v>
+        <v>197.10024950500002</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -4858,11 +4038,11 @@
       </c>
       <c r="K27" s="5">
         <f t="shared" si="0"/>
-        <v>-16.727694659000036</v>
+        <v>3.7454428584999846</v>
       </c>
       <c r="L27" s="5">
         <f>K27/io_1!$J$2*1000</f>
-        <v>-101.41500190368815</v>
+        <v>22.707498096311966</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="1"/>
@@ -4903,11 +4083,11 @@
       </c>
       <c r="K28" s="5">
         <f t="shared" si="0"/>
-        <v>-28.494254639000047</v>
+        <v>-8.0211171215000263</v>
       </c>
       <c r="L28" s="5">
         <f>K28/io_1!$J$2*1000</f>
-        <v>-172.752130366248</v>
+        <v>-48.629630366247895</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="1"/>
@@ -4934,7 +4114,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D29">
-        <v>706.96299999999997</v>
+        <v>876.69799999999998</v>
       </c>
       <c r="F29">
         <v>24.315000000000001</v>
@@ -4944,15 +4124,15 @@
       </c>
       <c r="J29" s="5">
         <f>B29+(C29+H29+E29)/1000*io_1!$J$1+(D29+F29*2+G29*2)/1000*io_1!$J$2</f>
-        <v>181.08888491300002</v>
+        <v>209.08548501799999</v>
       </c>
       <c r="K29" s="5">
         <f t="shared" si="0"/>
-        <v>2.8458467399999847</v>
+        <v>-4.6776158474999647</v>
       </c>
       <c r="L29" s="5">
         <f>K29/io_1!$J$2*1000</f>
-        <v>17.253516305632761</v>
+        <v>-28.35898369436693</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="1"/>
@@ -4964,7 +4144,7 @@
       </c>
       <c r="S29">
         <f t="shared" si="3"/>
-        <v>181.08888491300002</v>
+        <v>209.08548501799999</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
@@ -4993,11 +4173,11 @@
       </c>
       <c r="K30" s="5">
         <f t="shared" si="0"/>
-        <v>-16.082700511000013</v>
+        <v>4.390437006500008</v>
       </c>
       <c r="L30" s="5">
         <f>K30/io_1!$J$2*1000</f>
-        <v>-97.504595593629375</v>
+        <v>26.617904406370734</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="1"/>
@@ -5018,7 +4198,7 @@
       </c>
       <c r="C31" s="9">
         <f>MAX(J8:J30)-MIN(J8:J30)</f>
-        <v>76.442551184000052</v>
+        <v>15.328736787000025</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -5030,7 +4210,7 @@
       </c>
       <c r="C32" s="6">
         <f>T9-T8</f>
-        <v>76.442551184000052</v>
+        <v>15.328736787000025</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
@@ -6234,76 +5414,76 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:K30">
-    <cfRule type="cellIs" dxfId="34" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="between">
       <formula>-$Q$4*$Q$2</formula>
       <formula>$Q$4*$Q$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:J46">
-    <cfRule type="cellIs" dxfId="33" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>$O$36</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>$O$37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:K46">
-    <cfRule type="cellIs" dxfId="31" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="between">
       <formula>-$Q$4*$Q$1</formula>
       <formula>$Q$4*$Q$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L36:L46">
-    <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>$O$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>$O$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48">
-    <cfRule type="cellIs" dxfId="28" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
       <formula>$J$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:J30">
-    <cfRule type="cellIs" dxfId="26" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>$O$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>$O$8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52:J62">
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>$O$52</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>$O$53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:K62">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>-$Q$4*$Q$1</formula>
       <formula>$Q$4*$Q$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52:L62">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>$O$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>$O$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>$J$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
All DDR3 traces tuned to match their respective clock groups by 10ps.
</commit_message>
<xml_diff>
--- a/DDR3 board timings.xlsx
+++ b/DDR3 board timings.xlsx
@@ -2882,8 +2882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3125,7 +3125,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D8">
-        <v>372.54899999999998</v>
+        <v>379.072</v>
       </c>
       <c r="E8">
         <v>385.08300000000003</v>
@@ -3141,15 +3141,15 @@
       </c>
       <c r="J8" s="5">
         <f>B8+(C8+H8+E8)/1000*io_1!$J$1+(D8+F8*2+G8*2)/1000*io_1!$J$2</f>
-        <v>208.54384728199997</v>
+        <v>209.61977047099998</v>
       </c>
       <c r="K8" s="5">
         <f>$J$4-J8</f>
-        <v>-4.1359781114999521</v>
+        <v>-5.2119013004999601</v>
       </c>
       <c r="L8" s="5">
         <f>K8/io_1!$J$2*1000</f>
-        <v>-25.075196349647765</v>
+        <v>-31.598196349647818</v>
       </c>
       <c r="M8" t="str">
         <f>IF(J8=$R$8, "Route","")</f>
@@ -3172,7 +3172,7 @@
       </c>
       <c r="S8">
         <f>IF(D8=0,"",J8)</f>
-        <v>208.54384728199997</v>
+        <v>209.61977047099998</v>
       </c>
       <c r="T8">
         <f>MIN(S8:S30)</f>
@@ -3571,7 +3571,7 @@
         <v>365.91</v>
       </c>
       <c r="E17">
-        <v>447.46800000000002</v>
+        <v>486.83800000000002</v>
       </c>
       <c r="F17">
         <v>9.0549999999999997</v>
@@ -3584,15 +3584,15 @@
       </c>
       <c r="J17" s="5">
         <f>B17+(C17+H17+E17)/1000*io_1!$J$1+(D17+F17*2+G17*2)/1000*io_1!$J$2</f>
-        <v>198.44337526000001</v>
+        <v>204.28064705000003</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="0"/>
-        <v>5.9644939105000105</v>
+        <v>0.12722212049999371</v>
       </c>
       <c r="L17" s="5">
         <f>K17/io_1!$J$2*1000</f>
-        <v>36.160939903481868</v>
+        <v>0.77130960695509176</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="1"/>
@@ -3604,7 +3604,7 @@
       </c>
       <c r="S17">
         <f t="shared" si="3"/>
-        <v>198.44337526000001</v>
+        <v>204.28064705000003</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
@@ -3619,7 +3619,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D18">
-        <v>883.68399999999997</v>
+        <v>868.49599999999998</v>
       </c>
       <c r="F18">
         <v>27.895</v>
@@ -3629,15 +3629,15 @@
       </c>
       <c r="J18" s="5">
         <f>B18+(C18+H18+E18)/1000*io_1!$J$1+(D18+F18*2+G18*2)/1000*io_1!$J$2</f>
-        <v>204.677268696</v>
+        <v>202.17211441199998</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="0"/>
-        <v>-0.2693995254999777</v>
+        <v>2.2357547585000361</v>
       </c>
       <c r="L18" s="5">
         <f>K18/io_1!$J$2*1000</f>
-        <v>-1.6332886239487439</v>
+        <v>13.554711376051339</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="1"/>
@@ -3649,7 +3649,7 @@
       </c>
       <c r="S18">
         <f t="shared" si="3"/>
-        <v>204.677268696</v>
+        <v>202.17211441199998</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
@@ -3799,7 +3799,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D22">
-        <v>809.48900000000003</v>
+        <v>816.01199999999994</v>
       </c>
       <c r="F22">
         <v>27.895</v>
@@ -3809,15 +3809,15 @@
       </c>
       <c r="J22" s="5">
         <f>B22+(C22+H22+E22)/1000*io_1!$J$1+(D22+F22*2+G22*2)/1000*io_1!$J$2</f>
-        <v>200.51682281100003</v>
+        <v>201.59274600000001</v>
       </c>
       <c r="K22" s="5">
         <f t="shared" si="0"/>
-        <v>3.8910463594999953</v>
+        <v>2.8151231705000157</v>
       </c>
       <c r="L22" s="5">
         <f>K22/io_1!$J$2*1000</f>
-        <v>23.590248507059986</v>
+        <v>17.067248507060111</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="1"/>
@@ -3829,7 +3829,7 @@
       </c>
       <c r="S22">
         <f t="shared" si="3"/>
-        <v>200.51682281100003</v>
+        <v>201.59274600000001</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
@@ -3889,7 +3889,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D24">
-        <v>841.94</v>
+        <v>848.46299999999997</v>
       </c>
       <c r="F24">
         <v>27.895</v>
@@ -3899,15 +3899,15 @@
       </c>
       <c r="J24" s="5">
         <f>B24+(C24+H24+E24)/1000*io_1!$J$1+(D24+F24*2+G24*2)/1000*io_1!$J$2</f>
-        <v>203.992888104</v>
+        <v>205.06881129299998</v>
       </c>
       <c r="K24" s="5">
         <f t="shared" si="0"/>
-        <v>0.41498106650001887</v>
+        <v>-0.66094212249996076</v>
       </c>
       <c r="L24" s="5">
         <f>K24/io_1!$J$2*1000</f>
-        <v>2.5159058977951103</v>
+        <v>-4.0070941022047659</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="1"/>
@@ -3919,7 +3919,7 @@
       </c>
       <c r="S24">
         <f t="shared" si="3"/>
-        <v>203.992888104</v>
+        <v>205.06881129299998</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
@@ -4273,7 +4273,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D36">
-        <v>465.80200000000002</v>
+        <v>612.30999999999995</v>
       </c>
       <c r="F36">
         <v>9.0549999999999997</v>
@@ -4283,15 +4283,15 @@
       </c>
       <c r="J36" s="5">
         <f>B36+(C36+H36+E36)/1000*io_1!$J$1+(D36+F36*2+G36*2)/1000*io_1!$J$2</f>
-        <v>146.10300573000001</v>
+        <v>170.26847477400003</v>
       </c>
       <c r="K36" s="5">
         <f>$F$48-J36</f>
-        <v>16.252937433000028</v>
+        <v>4.2490456649999828</v>
       </c>
       <c r="L36" s="5">
         <f>K36/io_1!$J$2*1000</f>
-        <v>98.53669105691074</v>
+        <v>25.760691056910463</v>
       </c>
       <c r="M36" t="str">
         <f>IF(J36=$R$36, "Route","")</f>
@@ -4302,7 +4302,7 @@
       </c>
       <c r="O36" s="5">
         <f>MIN(J36:J46)</f>
-        <v>142.18855371000001</v>
+        <v>168.92994562700002</v>
       </c>
       <c r="Q36">
         <f>IF(D36=0,J36,0)</f>
@@ -4314,11 +4314,11 @@
       </c>
       <c r="S36">
         <f>IF(D36=0,"",J36)</f>
-        <v>146.10300573000001</v>
+        <v>170.26847477400003</v>
       </c>
       <c r="T36">
         <f>MIN(S36:S46)</f>
-        <v>142.18855371000001</v>
+        <v>168.92994562700002</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
@@ -4333,7 +4333,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D37">
-        <v>571.98599999999999</v>
+        <v>632.27599999999995</v>
       </c>
       <c r="F37">
         <v>12.635</v>
@@ -4343,15 +4343,15 @@
       </c>
       <c r="J37" s="5">
         <f>B37+(C37+H37+E37)/1000*io_1!$J$1+(D37+F37*2+G37*2)/1000*io_1!$J$2</f>
-        <v>162.33530512200002</v>
+        <v>172.27971859199999</v>
       </c>
       <c r="K37" s="5">
         <f t="shared" ref="K37:K46" si="4">$F$48-J37</f>
-        <v>2.0638041000012208E-2</v>
+        <v>2.2378018470000143</v>
       </c>
       <c r="L37" s="5">
         <f>K37/io_1!$J$2*1000</f>
-        <v>0.12512226041730906</v>
+        <v>13.567122260417321</v>
       </c>
       <c r="M37" t="str">
         <f t="shared" ref="M37:M46" si="5">IF(J37=$R$36, "Route","")</f>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="O37" s="5">
         <f>MAX(J36:J46)</f>
-        <v>183.47388644400002</v>
+        <v>181.34909071800001</v>
       </c>
       <c r="Q37">
         <f t="shared" ref="Q37:Q46" si="6">IF(D37=0,J37,0)</f>
@@ -4370,11 +4370,11 @@
       </c>
       <c r="S37">
         <f t="shared" ref="S37:S46" si="7">IF(D37=0,"",J37)</f>
-        <v>162.33530512200002</v>
+        <v>172.27971859199999</v>
       </c>
       <c r="T37">
         <f>MAX(S36:S46)</f>
-        <v>183.47388644400002</v>
+        <v>181.34909071800001</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
@@ -4389,7 +4389,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D38">
-        <v>371.31400000000002</v>
+        <v>518.77800000000002</v>
       </c>
       <c r="F38">
         <v>9.0549999999999997</v>
@@ -4399,15 +4399,15 @@
       </c>
       <c r="J38" s="5">
         <f>B38+(C38+H38+E38)/1000*io_1!$J$1+(D38+F38*2+G38*2)/1000*io_1!$J$2</f>
-        <v>146.242871546</v>
+        <v>170.56602609800001</v>
       </c>
       <c r="K38" s="5">
         <f t="shared" si="4"/>
-        <v>16.113071617000031</v>
+        <v>3.9514943410000001</v>
       </c>
       <c r="L38" s="5">
         <f>K38/io_1!$J$2*1000</f>
-        <v>97.688726511582971</v>
+        <v>23.956726511582787</v>
       </c>
       <c r="M38" t="str">
         <f t="shared" si="5"/>
@@ -4419,7 +4419,7 @@
       </c>
       <c r="S38">
         <f t="shared" si="7"/>
-        <v>146.242871546</v>
+        <v>170.56602609800001</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
@@ -4434,7 +4434,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D39">
-        <v>589.48</v>
+        <v>576.59799999999996</v>
       </c>
       <c r="F39">
         <v>24.315000000000001</v>
@@ -4444,15 +4444,15 @@
       </c>
       <c r="J39" s="5">
         <f>B39+(C39+H39+E39)/1000*io_1!$J$1+(D39+F39*2+G39*2)/1000*io_1!$J$2</f>
-        <v>183.47388644400002</v>
+        <v>181.34909071800001</v>
       </c>
       <c r="K39" s="5">
         <f t="shared" si="4"/>
-        <v>-21.117943280999981</v>
+        <v>-6.8315702790000046</v>
       </c>
       <c r="L39" s="5">
         <f>K39/io_1!$J$2*1000</f>
-        <v>-128.03176419126595</v>
+        <v>-41.417764191266095</v>
       </c>
       <c r="M39" t="str">
         <f t="shared" si="5"/>
@@ -4464,7 +4464,7 @@
       </c>
       <c r="S39">
         <f t="shared" si="7"/>
-        <v>183.47388644400002</v>
+        <v>181.34909071800001</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
@@ -4479,7 +4479,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D40">
-        <v>407.98200000000003</v>
+        <v>581.77</v>
       </c>
       <c r="F40">
         <v>27.895</v>
@@ -4489,15 +4489,15 @@
       </c>
       <c r="J40" s="5">
         <f>B40+(C40+H40+E40)/1000*io_1!$J$1+(D40+F40*2+G40*2)/1000*io_1!$J$2</f>
-        <v>142.18855371000001</v>
+        <v>170.85366779399999</v>
       </c>
       <c r="K40" s="5">
         <f t="shared" si="4"/>
-        <v>20.167389453000027</v>
+        <v>3.6638526450000199</v>
       </c>
       <c r="L40" s="5">
         <f>K40/io_1!$J$2*1000</f>
-        <v>122.26884107237061</v>
+        <v>22.212841072370576</v>
       </c>
       <c r="M40" t="str">
         <f t="shared" si="5"/>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="S40">
         <f t="shared" si="7"/>
-        <v>142.18855371000001</v>
+        <v>170.85366779399999</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
@@ -4524,7 +4524,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D41">
-        <v>510.34399999999999</v>
+        <v>570.63400000000001</v>
       </c>
       <c r="F41">
         <v>12.635</v>
@@ -4534,15 +4534,15 @@
       </c>
       <c r="J41" s="5">
         <f>B41+(C41+H41+E41)/1000*io_1!$J$1+(D41+F41*2+G41*2)/1000*io_1!$J$2</f>
-        <v>164.75488871600004</v>
+        <v>174.69930218600001</v>
       </c>
       <c r="K41" s="5">
         <f t="shared" si="4"/>
-        <v>-2.3989455530000043</v>
+        <v>-0.18178174700000227</v>
       </c>
       <c r="L41" s="5">
         <f>K41/io_1!$J$2*1000</f>
-        <v>-14.544088278981249</v>
+        <v>-1.1020882789812374</v>
       </c>
       <c r="M41" t="str">
         <f t="shared" si="5"/>
@@ -4554,7 +4554,7 @@
       </c>
       <c r="S41">
         <f t="shared" si="7"/>
-        <v>164.75488871600004</v>
+        <v>174.69930218600001</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
@@ -4569,7 +4569,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D42">
-        <v>465.80200000000002</v>
+        <v>552.976</v>
       </c>
       <c r="F42">
         <v>12.635</v>
@@ -4579,15 +4579,15 @@
       </c>
       <c r="J42" s="5">
         <f>B42+(C42+H42+E42)/1000*io_1!$J$1+(D42+F42*2+G42*2)/1000*io_1!$J$2</f>
-        <v>159.95699761000003</v>
+        <v>174.33573869200001</v>
       </c>
       <c r="K42" s="5">
         <f t="shared" si="4"/>
-        <v>2.3989455530000043</v>
+        <v>0.18178174700000227</v>
       </c>
       <c r="L42" s="5">
         <f>K42/io_1!$J$2*1000</f>
-        <v>14.544088278981249</v>
+        <v>1.1020882789812374</v>
       </c>
       <c r="M42" t="str">
         <f t="shared" si="5"/>
@@ -4599,7 +4599,7 @@
       </c>
       <c r="S42">
         <f t="shared" si="7"/>
-        <v>159.95699761000003</v>
+        <v>174.33573869200001</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
@@ -4614,7 +4614,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D43">
-        <v>445.04599999999999</v>
+        <v>584.07600000000002</v>
       </c>
       <c r="F43">
         <v>27.895</v>
@@ -4624,15 +4624,15 @@
       </c>
       <c r="J43" s="5">
         <f>B43+(C43+H43+E43)/1000*io_1!$J$1+(D43+F43*2+G43*2)/1000*io_1!$J$2</f>
-        <v>153.33700106200001</v>
+        <v>176.26902635200003</v>
       </c>
       <c r="K43" s="5">
         <f t="shared" si="4"/>
-        <v>9.0189421010000217</v>
+        <v>-1.7515059130000168</v>
       </c>
       <c r="L43" s="5">
         <f>K43/io_1!$J$2*1000</f>
-        <v>54.679144316521594</v>
+        <v>-10.618855683478637</v>
       </c>
       <c r="M43" t="str">
         <f t="shared" si="5"/>
@@ -4644,7 +4644,7 @@
       </c>
       <c r="S43">
         <f t="shared" si="7"/>
-        <v>153.33700106200001</v>
+        <v>176.26902635200003</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
@@ -4659,7 +4659,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D44">
-        <v>510.34399999999999</v>
+        <v>576.202</v>
       </c>
       <c r="F44">
         <v>24.315000000000001</v>
@@ -4669,15 +4669,15 @@
       </c>
       <c r="J44" s="5">
         <f>B44+(C44+H44+E44)/1000*io_1!$J$1+(D44+F44*2+G44*2)/1000*io_1!$J$2</f>
-        <v>158.27545719600002</v>
+        <v>169.13827329</v>
       </c>
       <c r="K44" s="5">
         <f t="shared" si="4"/>
-        <v>4.0804859670000155</v>
+        <v>5.3792471490000082</v>
       </c>
       <c r="L44" s="5">
         <f>K44/io_1!$J$2*1000</f>
-        <v>24.73876410032566</v>
+        <v>32.612764100325613</v>
       </c>
       <c r="M44" t="str">
         <f t="shared" si="5"/>
@@ -4689,7 +4689,7 @@
       </c>
       <c r="S44">
         <f t="shared" si="7"/>
-        <v>158.27545719600002</v>
+        <v>169.13827329</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
@@ -4704,7 +4704,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D45">
-        <v>595.60699999999997</v>
+        <v>651.68100000000004</v>
       </c>
       <c r="F45">
         <v>9.0549999999999997</v>
@@ -4714,15 +4714,15 @@
       </c>
       <c r="J45" s="5">
         <f>B45+(C45+H45+E45)/1000*io_1!$J$1+(D45+F45*2+G45*2)/1000*io_1!$J$2</f>
-        <v>159.680931845</v>
+        <v>168.92994562700002</v>
       </c>
       <c r="K45" s="5">
         <f t="shared" si="4"/>
-        <v>2.6750113180000312</v>
+        <v>5.5875748119999855</v>
       </c>
       <c r="L45" s="5">
         <f>K45/io_1!$J$2*1000</f>
-        <v>16.217792316133643</v>
+        <v>33.875792316133364</v>
       </c>
       <c r="M45" t="str">
         <f t="shared" si="5"/>
@@ -4734,7 +4734,7 @@
       </c>
       <c r="S45">
         <f t="shared" si="7"/>
-        <v>159.680931845</v>
+        <v>168.92994562700002</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
@@ -4749,7 +4749,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D46">
-        <v>447.35199999999998</v>
+        <v>553.53599999999994</v>
       </c>
       <c r="F46">
         <v>27.895</v>
@@ -4759,15 +4759,15 @@
       </c>
       <c r="J46" s="5">
         <f>B46+(C46+H46+E46)/1000*io_1!$J$1+(D46+F46*2+G46*2)/1000*io_1!$J$2</f>
-        <v>156.97185962</v>
+        <v>174.48616713199999</v>
       </c>
       <c r="K46" s="5">
         <f t="shared" si="4"/>
-        <v>5.3840835430000311</v>
+        <v>3.1353307000017594E-2</v>
       </c>
       <c r="L46" s="5">
         <f>K46/io_1!$J$2*1000</f>
-        <v>32.642085708396422</v>
+        <v>0.19008570839634051</v>
       </c>
       <c r="M46" t="str">
         <f t="shared" si="5"/>
@@ -4779,7 +4779,7 @@
       </c>
       <c r="S46">
         <f t="shared" si="7"/>
-        <v>156.97185962</v>
+        <v>174.48616713199999</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
@@ -4788,14 +4788,14 @@
       </c>
       <c r="C47" s="9">
         <f>MAX(J36:J46)-MIN(J36:J46)</f>
-        <v>41.285332734000008</v>
+        <v>12.41914509099999</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>185</v>
       </c>
       <c r="F47" s="5">
         <f>MAX(J41:J42)-MIN(J41:J42)</f>
-        <v>4.7978911060000087</v>
+        <v>0.36356349400000454</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.3">
@@ -4804,14 +4804,14 @@
       </c>
       <c r="C48" s="6">
         <f>T37-T36</f>
-        <v>41.285332734000008</v>
+        <v>12.41914509099999</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>186</v>
       </c>
       <c r="F48" s="5">
         <f>AVERAGE(J41:J42)</f>
-        <v>162.35594316300003</v>
+        <v>174.51752043900001</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.3">
@@ -4871,7 +4871,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D52">
-        <v>402.81</v>
+        <v>474.23599999999999</v>
       </c>
       <c r="F52">
         <v>12.635</v>
@@ -4881,15 +4881,15 @@
       </c>
       <c r="J52" s="5">
         <f>B52+(C52+H52+E52)/1000*io_1!$J$1+(D52+F52*2+G52*2)/1000*io_1!$J$2</f>
-        <v>142.90440815400001</v>
+        <v>154.685626872</v>
       </c>
       <c r="K52" s="5">
         <f>$F$64-J52</f>
-        <v>2.6162656320000224</v>
+        <v>2.7276021570000069</v>
       </c>
       <c r="L52" s="5">
         <f>K52/io_1!$J$2*1000</f>
-        <v>15.861634819301349</v>
+        <v>16.536634819301252</v>
       </c>
       <c r="M52" t="str">
         <f>IF(J52=$R$52, "Route","")</f>
@@ -4900,7 +4900,7 @@
       </c>
       <c r="O52" s="5">
         <f>MIN(J52:J62)</f>
-        <v>142.90440815400001</v>
+        <v>151.90009332100001</v>
       </c>
       <c r="Q52">
         <f>IF(D52=0,J52,0)</f>
@@ -4912,11 +4912,11 @@
       </c>
       <c r="S52">
         <f>IF(D52=0,"",J52)</f>
-        <v>142.90440815400001</v>
+        <v>154.685626872</v>
       </c>
       <c r="T52">
         <f>MIN(S52:S62)</f>
-        <v>142.90440815400001</v>
+        <v>151.90009332100001</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.3">
@@ -4945,11 +4945,11 @@
       </c>
       <c r="K53" s="5">
         <f t="shared" ref="K53:K62" si="8">$F$64-J53</f>
-        <v>-6.9596411059999923</v>
+        <v>4.9329141369999832</v>
       </c>
       <c r="L53" s="5">
         <f>K53/io_1!$J$2*1000</f>
-        <v>-42.19421925149895</v>
+        <v>29.906780748500893</v>
       </c>
       <c r="M53" t="str">
         <f t="shared" ref="M53:M62" si="9">IF(J53=$R$52, "Route","")</f>
@@ -5001,11 +5001,11 @@
       </c>
       <c r="K54" s="5">
         <f t="shared" si="8"/>
-        <v>-8.5118319439999937</v>
+        <v>3.3807232989999818</v>
       </c>
       <c r="L54" s="5">
         <f>K54/io_1!$J$2*1000</f>
-        <v>-51.604687340475152</v>
+        <v>20.496312659524694</v>
       </c>
       <c r="M54" t="str">
         <f t="shared" si="9"/>
@@ -5046,11 +5046,11 @@
       </c>
       <c r="K55" s="5">
         <f t="shared" si="8"/>
-        <v>-16.084466127999974</v>
+        <v>-4.1919108849999986</v>
       </c>
       <c r="L55" s="5">
         <f>K55/io_1!$J$2*1000</f>
-        <v>-97.515300000606118</v>
+        <v>-25.414300000606257</v>
       </c>
       <c r="M55" t="str">
         <f t="shared" si="9"/>
@@ -5091,11 +5091,11 @@
       </c>
       <c r="K56" s="5">
         <f t="shared" si="8"/>
-        <v>-10.115287215999984</v>
+        <v>1.777268026999991</v>
       </c>
       <c r="L56" s="5">
         <f>K56/io_1!$J$2*1000</f>
-        <v>-61.325956336431275</v>
+        <v>10.775043663568571</v>
       </c>
       <c r="M56" t="str">
         <f t="shared" si="9"/>
@@ -5122,7 +5122,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D57">
-        <v>371.31400000000002</v>
+        <v>439.47800000000001</v>
       </c>
       <c r="F57">
         <v>27.895</v>
@@ -5132,15 +5132,15 @@
       </c>
       <c r="J57" s="5">
         <f>B57+(C57+H57+E57)/1000*io_1!$J$1+(D57+F57*2+G57*2)/1000*io_1!$J$2</f>
-        <v>146.32392378600002</v>
+        <v>157.56709843800002</v>
       </c>
       <c r="K57" s="5">
         <f t="shared" si="8"/>
-        <v>-0.80324999999999136</v>
+        <v>-0.15386940900000923</v>
       </c>
       <c r="L57" s="5">
         <f>K57/io_1!$J$2*1000</f>
-        <v>-4.8698641348829064</v>
+        <v>-0.93286413488301534</v>
       </c>
       <c r="M57" t="str">
         <f t="shared" si="9"/>
@@ -5152,7 +5152,7 @@
       </c>
       <c r="S57">
         <f t="shared" si="11"/>
-        <v>146.32392378600002</v>
+        <v>157.56709843800002</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.3">
@@ -5167,7 +5167,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D58">
-        <v>371.31400000000002</v>
+        <v>447.35199999999998</v>
       </c>
       <c r="F58">
         <v>27.895</v>
@@ -5177,15 +5177,15 @@
       </c>
       <c r="J58" s="5">
         <f>B58+(C58+H58+E58)/1000*io_1!$J$1+(D58+F58*2+G58*2)/1000*io_1!$J$2</f>
-        <v>144.71742378600004</v>
+        <v>157.25935962</v>
       </c>
       <c r="K58" s="5">
         <f t="shared" si="8"/>
-        <v>0.80324999999999136</v>
+        <v>0.15386940900000923</v>
       </c>
       <c r="L58" s="5">
         <f>K58/io_1!$J$2*1000</f>
-        <v>4.8698641348829064</v>
+        <v>0.93286413488301534</v>
       </c>
       <c r="M58" t="str">
         <f t="shared" si="9"/>
@@ -5197,7 +5197,7 @@
       </c>
       <c r="S58">
         <f t="shared" si="11"/>
-        <v>144.71742378600004</v>
+        <v>157.25935962</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.3">
@@ -5212,25 +5212,25 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D59">
-        <v>371.31400000000002</v>
+        <v>425.08100000000002</v>
       </c>
       <c r="F59">
-        <v>12.635</v>
+        <v>24.315000000000001</v>
       </c>
       <c r="H59">
         <v>22.271000000000001</v>
       </c>
       <c r="J59" s="5">
         <f>B59+(C59+H59+E59)/1000*io_1!$J$1+(D59+F59*2+G59*2)/1000*io_1!$J$2</f>
-        <v>143.53836342599999</v>
+        <v>156.25992218700003</v>
       </c>
       <c r="K59" s="5">
         <f t="shared" si="8"/>
-        <v>1.9823103600000422</v>
+        <v>1.1533068419999779</v>
       </c>
       <c r="L59" s="5">
         <f>K59/io_1!$J$2*1000</f>
-        <v>12.018153907713829</v>
+        <v>6.9921539077134396</v>
       </c>
       <c r="M59" t="str">
         <f t="shared" si="9"/>
@@ -5242,7 +5242,7 @@
       </c>
       <c r="S59">
         <f t="shared" si="11"/>
-        <v>143.53836342599999</v>
+        <v>156.25992218700003</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.3">
@@ -5271,11 +5271,11 @@
       </c>
       <c r="K60" s="5">
         <f t="shared" si="8"/>
-        <v>-10.061518113999966</v>
+        <v>1.8310371290000091</v>
       </c>
       <c r="L60" s="5">
         <f>K60/io_1!$J$2*1000</f>
-        <v>-60.999970377645404</v>
+        <v>11.101029622354444</v>
       </c>
       <c r="M60" t="str">
         <f t="shared" si="9"/>
@@ -5316,11 +5316,11 @@
       </c>
       <c r="K61" s="5">
         <f t="shared" si="8"/>
-        <v>-6.3794195349999825</v>
+        <v>5.513135707999993</v>
       </c>
       <c r="L61" s="5">
         <f>K61/io_1!$J$2*1000</f>
-        <v>-38.676509673038453</v>
+        <v>33.42449032696139</v>
       </c>
       <c r="M61" t="str">
         <f t="shared" si="9"/>
@@ -5361,11 +5361,11 @@
       </c>
       <c r="K62" s="5">
         <f t="shared" si="8"/>
-        <v>-9.4854213999999786</v>
+        <v>2.4071338429999969</v>
       </c>
       <c r="L62" s="5">
         <f>K62/io_1!$J$2*1000</f>
-        <v>-57.507268571567018</v>
+        <v>14.593731428432832</v>
       </c>
       <c r="M62" t="str">
         <f t="shared" si="9"/>
@@ -5386,14 +5386,14 @@
       </c>
       <c r="C63" s="9">
         <f>MAX(J52:J62)-MIN(J52:J62)</f>
-        <v>18.700731759999996</v>
+        <v>9.7050465929999916</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>185</v>
       </c>
       <c r="F63" s="5">
         <f>MAX(J57:J58)-MIN(J57:J58)</f>
-        <v>1.6064999999999827</v>
+        <v>0.30773881800001845</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.3">
@@ -5402,14 +5402,14 @@
       </c>
       <c r="C64" s="6">
         <f>T53-T52</f>
-        <v>18.700731759999996</v>
+        <v>9.7050465929999916</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>186</v>
       </c>
       <c r="F64" s="5">
         <f>AVERAGE(J57:J58)</f>
-        <v>145.52067378600003</v>
+        <v>157.41322902900001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All IPMI signals and peripherals routed and timed. Only GPIOs and power missing.
</commit_message>
<xml_diff>
--- a/DDR3 board timings.xlsx
+++ b/DDR3 board timings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16548" windowHeight="6036" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16548" windowHeight="6036" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Pin delays - All" sheetId="4" r:id="rId1"/>
@@ -3870,47 +3870,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -16790,76 +16750,76 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:K30">
-    <cfRule type="cellIs" dxfId="31" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="24" operator="between">
       <formula>-$Q$4*$Q$2</formula>
       <formula>$Q$4*$Q$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:J46">
-    <cfRule type="cellIs" dxfId="30" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
       <formula>$O$36</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
       <formula>$O$37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:K46">
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="14" operator="between">
       <formula>-$Q$4*$Q$1</formula>
       <formula>$Q$4*$Q$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L36:L46">
-    <cfRule type="cellIs" dxfId="27" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
       <formula>$O$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="13" operator="equal">
       <formula>$O$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48">
-    <cfRule type="cellIs" dxfId="25" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="10" operator="lessThan">
       <formula>$J$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="greaterThan">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:J30">
-    <cfRule type="cellIs" dxfId="23" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>$O$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>$O$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52:J62">
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
       <formula>$O$52</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>$O$53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:K62">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="between">
       <formula>-$Q$4*$Q$1</formula>
       <formula>$Q$4*$Q$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52:L62">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>$O$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>$O$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="lessThan">
       <formula>$J$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="greaterThan">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16873,7 +16833,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16933,14 +16893,14 @@
         <v>1202.3019999999999</v>
       </c>
       <c r="F2" s="14">
-        <v>9.0549999999999997</v>
+        <v>27.895</v>
       </c>
       <c r="H2">
         <v>45.079000000000001</v>
       </c>
       <c r="J2" s="5">
         <f>B2+(C2+H2+E2)/1000*io_1!$J$1+(D2+F2*2+G2*2)/1000*io_1!$J$2</f>
-        <v>311.59919896599996</v>
+        <v>317.81425120599999</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>1049</v>
@@ -16976,11 +16936,11 @@
       </c>
       <c r="K3" s="5">
         <f>$J$2-J3</f>
-        <v>-30.99478761000006</v>
+        <v>-24.779735370000026</v>
       </c>
       <c r="L3" s="5">
         <f>K3/io_1!$J$2*1000</f>
-        <v>-187.91211272985248</v>
+        <v>-150.23211272985228</v>
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="5"/>
@@ -16996,25 +16956,25 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D4">
-        <v>1167.4290000000001</v>
+        <v>1126.1479999999999</v>
       </c>
       <c r="F4" s="14">
         <v>27.895</v>
       </c>
       <c r="H4">
-        <v>46.26</v>
+        <v>24.448</v>
       </c>
       <c r="J4" s="5">
         <f>B4+(C4+H4+E4)/1000*io_1!$J$1+(D4+F4*2+G4*2)/1000*io_1!$J$2</f>
-        <v>353.736297294</v>
+        <v>343.69328550699998</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" ref="K4:K6" si="0">$J$2-J4</f>
-        <v>-42.137098328000036</v>
+        <v>-25.87903430099999</v>
       </c>
       <c r="L4" s="5">
         <f>K4/io_1!$J$2*1000</f>
-        <v>-255.46460491200011</v>
+        <v>-156.89683285134859</v>
       </c>
       <c r="N4" s="8"/>
     </row>
@@ -17043,11 +17003,11 @@
       </c>
       <c r="K5" s="5">
         <f t="shared" si="0"/>
-        <v>23.158762641999942</v>
+        <v>29.373814881999976</v>
       </c>
       <c r="L5" s="5">
         <f>K5/io_1!$J$2*1000</f>
-        <v>140.40464064555599</v>
+        <v>178.08464064555619</v>
       </c>
       <c r="N5" s="8"/>
     </row>
@@ -17062,7 +17022,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D6">
-        <v>1179.24</v>
+        <v>1165.402</v>
       </c>
       <c r="F6" s="14">
         <v>27.895</v>
@@ -17072,15 +17032,15 @@
       </c>
       <c r="J6" s="5">
         <f>B6+(C6+H6+E6)/1000*io_1!$J$1+(D6+F6*2+G6*2)/1000*io_1!$J$2</f>
-        <v>307.76879928200003</v>
+        <v>305.48631804800004</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="0"/>
-        <v>3.8303996839999286</v>
+        <v>12.327933157999951</v>
       </c>
       <c r="L6" s="5">
         <f>K6/io_1!$J$2*1000</f>
-        <v>23.222565880333985</v>
+        <v>74.740565880334117</v>
       </c>
       <c r="N6" s="8"/>
     </row>
@@ -17098,37 +17058,37 @@
         <v>1105.2280000000001</v>
       </c>
       <c r="F7" s="14">
-        <v>27.895</v>
+        <v>9.0549999999999997</v>
       </c>
       <c r="H7">
         <v>29.788</v>
       </c>
       <c r="J7" s="5">
         <f>B7+(C7+H7+E7)/1000*io_1!$J$1+(D7+F7*2+G7*2)/1000*io_1!$J$2</f>
-        <v>312.35542372700002</v>
+        <v>306.14037148699998</v>
       </c>
       <c r="K7" s="5">
         <f>$J$2-J7</f>
-        <v>-0.75622476100005542</v>
+        <v>11.673879719000013</v>
       </c>
       <c r="L7" s="5">
         <f>K7/io_1!$J$2*1000</f>
-        <v>-4.5847641973291093</v>
+        <v>70.77523580267129</v>
       </c>
       <c r="N7" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K2:K7">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="between">
       <formula>-$Q$4*$Q$2</formula>
       <formula>$Q$4*$Q$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J7">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>$O$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>$O$9</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17141,8 +17101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17612,7 +17572,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D14">
-        <v>1606.723</v>
+        <v>1505.876</v>
       </c>
       <c r="F14" s="14">
         <v>9.0549999999999997</v>
@@ -17625,34 +17585,34 @@
       </c>
       <c r="M14" s="5">
         <f>B14+(C14+J14+E14)/1000*io_1!$J$1+(D14+F14+G14+H14+I14+L14*31.496)/1000*io_1!$J$2</f>
-        <v>414.02578323799997</v>
+        <v>397.39177651700004</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="1"/>
-        <v>-31.184012759999916</v>
+        <v>-14.550006038999982</v>
       </c>
       <c r="O14" s="5">
         <f>N14/io_1!$J$2*1000</f>
-        <v>-189.05932813153584</v>
+        <v>-88.212328131536239</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N7">
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="between">
       <formula>-$T$4*$T$2</formula>
       <formula>$T$4*$T$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M7 M9:M14">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>$R$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>$R$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9:N14">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>-$T$4*$T$2</formula>
       <formula>$T$4*$T$2</formula>
     </cfRule>
@@ -17665,7 +17625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -18135,18 +18095,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K2:K9">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>$N$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>$N$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K18">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$N$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>$N$9</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
IPMC fully routed. Split planes added, planes drawn. Missing fab notes and silkscreen.
</commit_message>
<xml_diff>
--- a/DDR3 board timings.xlsx
+++ b/DDR3 board timings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16548" windowHeight="6036" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16548" windowHeight="6036" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pin delays - All" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="1087">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="1090">
   <si>
     <t>#Top: ios   Floorplan: io_1   Part: xc7z020clg484-1</t>
   </si>
@@ -3286,6 +3286,15 @@
   </si>
   <si>
     <t>NEEDS UPDATE ON GB_* LINES</t>
+  </si>
+  <si>
+    <t>ps/inch</t>
+  </si>
+  <si>
+    <t>ps/mil</t>
+  </si>
+  <si>
+    <t>mil</t>
   </si>
 </sst>
 </file>
@@ -12948,7 +12957,7 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D17"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14218,8 +14227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14527,7 +14536,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D9">
-        <v>828.26700000000005</v>
+        <v>831.529</v>
       </c>
       <c r="F9">
         <v>12.635</v>
@@ -14537,15 +14546,15 @@
       </c>
       <c r="J9" s="5">
         <f>B9+(C9+H9+E9)/1000*io_1!$J$1+(D9+F9*2+G9*2)/1000*io_1!$J$2</f>
-        <v>198.64856210500002</v>
+        <v>199.18660617100002</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" ref="K9:K30" si="0">$J$4-J9</f>
-        <v>5.7593070654999963</v>
+        <v>5.2212629994999986</v>
       </c>
       <c r="L9" s="5">
         <f>K9/io_1!$J$2*1000</f>
-        <v>34.916953526369689</v>
+        <v>31.654953526369706</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" ref="M9:M30" si="1">IF(J9=$R$8, "Route","")</f>
@@ -14564,7 +14573,7 @@
       </c>
       <c r="S9">
         <f t="shared" ref="S9:S30" si="3">IF(D9=0,"",J9)</f>
-        <v>198.64856210500002</v>
+        <v>199.18660617100002</v>
       </c>
       <c r="T9">
         <f>MAX(S8:S30)</f>
@@ -14628,7 +14637,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D11">
-        <v>888.46100000000001</v>
+        <v>874.06399999999996</v>
       </c>
       <c r="F11">
         <v>9.0549999999999997</v>
@@ -14638,15 +14647,15 @@
       </c>
       <c r="J11" s="5">
         <f>B11+(C11+H11+E11)/1000*io_1!$J$1+(D11+F11*2+G11*2)/1000*io_1!$J$2</f>
-        <v>199.97564916700003</v>
+        <v>197.60096479600003</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="0"/>
-        <v>4.4322200034999923</v>
+        <v>6.8069043744999931</v>
       </c>
       <c r="L11" s="5">
         <f>K11/io_1!$J$2*1000</f>
-        <v>26.871222201002723</v>
+        <v>41.268222201002729</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="1"/>
@@ -14658,7 +14667,7 @@
       </c>
       <c r="S11">
         <f t="shared" si="3"/>
-        <v>199.97564916700003</v>
+        <v>197.60096479600003</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
@@ -15450,7 +15459,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D29">
-        <v>876.69799999999998</v>
+        <v>860.55399999999997</v>
       </c>
       <c r="F29">
         <v>24.315000000000001</v>
@@ -15460,15 +15469,15 @@
       </c>
       <c r="J29" s="5">
         <f>B29+(C29+H29+E29)/1000*io_1!$J$1+(D29+F29*2+G29*2)/1000*io_1!$J$2</f>
-        <v>209.08548501799999</v>
+        <v>206.42264522600001</v>
       </c>
       <c r="K29" s="5">
         <f t="shared" si="0"/>
-        <v>-4.6776158474999647</v>
+        <v>-2.0147760554999934</v>
       </c>
       <c r="L29" s="5">
         <f>K29/io_1!$J$2*1000</f>
-        <v>-28.35898369436693</v>
+        <v>-12.214983694367104</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="1"/>
@@ -15480,7 +15489,7 @@
       </c>
       <c r="S29">
         <f t="shared" si="3"/>
-        <v>209.08548501799999</v>
+        <v>206.42264522600001</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
@@ -15495,7 +15504,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D30">
-        <v>625.52</v>
+        <v>652.404</v>
       </c>
       <c r="F30">
         <v>24.315000000000001</v>
@@ -15505,15 +15514,15 @@
       </c>
       <c r="J30" s="5">
         <f>B30+(C30+H30+E30)/1000*io_1!$J$1+(D30+F30*2+G30*2)/1000*io_1!$J$2</f>
-        <v>200.01743216400001</v>
+        <v>204.45175977600002</v>
       </c>
       <c r="K30" s="5">
         <f t="shared" si="0"/>
-        <v>4.390437006500008</v>
+        <v>-4.3890605499996127E-2</v>
       </c>
       <c r="L30" s="5">
         <f>K30/io_1!$J$2*1000</f>
-        <v>26.617904406370734</v>
+        <v>-0.26609559362929086</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="1"/>
@@ -15525,7 +15534,7 @@
       </c>
       <c r="S30">
         <f t="shared" si="3"/>
-        <v>200.01743216400001</v>
+        <v>204.45175977600002</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
@@ -16830,10 +16839,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16890,17 +16899,17 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D2">
-        <v>1202.3019999999999</v>
+        <v>3216.2840000000001</v>
       </c>
       <c r="F2" s="14">
         <v>27.895</v>
       </c>
       <c r="H2">
-        <v>45.079000000000001</v>
+        <v>54.994999999999997</v>
       </c>
       <c r="J2" s="5">
         <f>B2+(C2+H2+E2)/1000*io_1!$J$1+(D2+F2*2+G2*2)/1000*io_1!$J$2</f>
-        <v>317.81425120599999</v>
+        <v>651.47669980399996</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>1049</v>
@@ -16922,25 +16931,25 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D3">
-        <v>1189.1400000000001</v>
+        <v>2890.0239999999999</v>
       </c>
       <c r="F3" s="14">
         <v>27.895</v>
       </c>
       <c r="H3">
-        <v>32.087000000000003</v>
+        <v>58.192999999999998</v>
       </c>
       <c r="J3" s="5">
         <f>B3+(C3+H3+E3)/1000*io_1!$J$1+(D3+F3*2+G3*2)/1000*io_1!$J$2</f>
-        <v>342.59398657600002</v>
+        <v>627.01355449000005</v>
       </c>
       <c r="K3" s="5">
         <f>$J$2-J3</f>
-        <v>-24.779735370000026</v>
+        <v>24.463145313999917</v>
       </c>
       <c r="L3" s="5">
         <f>K3/io_1!$J$2*1000</f>
-        <v>-150.23211272985228</v>
+        <v>148.31272205549746</v>
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="5"/>
@@ -16956,7 +16965,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D4">
-        <v>1126.1479999999999</v>
+        <v>2819.9490000000001</v>
       </c>
       <c r="F4" s="14">
         <v>27.895</v>
@@ -16966,15 +16975,15 @@
       </c>
       <c r="J4" s="5">
         <f>B4+(C4+H4+E4)/1000*io_1!$J$1+(D4+F4*2+G4*2)/1000*io_1!$J$2</f>
-        <v>343.69328550699998</v>
+        <v>623.07390385000008</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" ref="K4:K6" si="0">$J$2-J4</f>
-        <v>-25.87903430099999</v>
+        <v>28.402795953999885</v>
       </c>
       <c r="L4" s="5">
         <f>K4/io_1!$J$2*1000</f>
-        <v>-156.89683285134859</v>
+        <v>172.19764375572097</v>
       </c>
       <c r="N4" s="8"/>
     </row>
@@ -16989,25 +16998,25 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D5">
-        <v>1186.5540000000001</v>
+        <v>3296.047</v>
       </c>
       <c r="F5" s="14">
         <v>27.895</v>
       </c>
       <c r="H5">
-        <v>26.725000000000001</v>
+        <v>34.484999999999999</v>
       </c>
       <c r="J5" s="5">
         <f>B5+(C5+H5+E5)/1000*io_1!$J$1+(D5+F5*2+G5*2)/1000*io_1!$J$2</f>
-        <v>288.44043632400002</v>
+        <v>637.53709214300011</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="0"/>
-        <v>29.373814881999976</v>
+        <v>13.939607660999854</v>
       </c>
       <c r="L5" s="5">
         <f>K5/io_1!$J$2*1000</f>
-        <v>178.08464064555619</v>
+        <v>84.511665611755902</v>
       </c>
       <c r="N5" s="8"/>
     </row>
@@ -17022,25 +17031,25 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D6">
-        <v>1165.402</v>
+        <v>3160.1619999999998</v>
       </c>
       <c r="F6" s="14">
         <v>27.895</v>
       </c>
       <c r="H6">
-        <v>30.905000000000001</v>
+        <v>32.853999999999999</v>
       </c>
       <c r="J6" s="5">
         <f>B6+(C6+H6+E6)/1000*io_1!$J$1+(D6+F6*2+G6*2)/1000*io_1!$J$2</f>
-        <v>305.48631804800004</v>
+        <v>634.79698911100002</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="0"/>
-        <v>12.327933157999951</v>
+        <v>16.679710692999947</v>
       </c>
       <c r="L6" s="5">
         <f>K6/io_1!$J$2*1000</f>
-        <v>74.740565880334117</v>
+        <v>101.12408949152099</v>
       </c>
       <c r="N6" s="8"/>
     </row>
@@ -17055,27 +17064,58 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D7">
-        <v>1105.2280000000001</v>
+        <v>3087.9450000000002</v>
       </c>
       <c r="F7" s="14">
-        <v>9.0549999999999997</v>
+        <v>27.895</v>
       </c>
       <c r="H7">
-        <v>29.788</v>
+        <v>37.070999999999998</v>
       </c>
       <c r="J7" s="5">
         <f>B7+(C7+H7+E7)/1000*io_1!$J$1+(D7+F7*2+G7*2)/1000*io_1!$J$2</f>
-        <v>306.14037148699998</v>
+        <v>640.47054241900003</v>
       </c>
       <c r="K7" s="5">
         <f>$J$2-J7</f>
-        <v>11.673879719000013</v>
+        <v>11.006157384999938</v>
       </c>
       <c r="L7" s="5">
         <f>K7/io_1!$J$2*1000</f>
-        <v>70.77523580267129</v>
+        <v>66.727035309167036</v>
       </c>
       <c r="N7" s="8"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C13" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>148.267</v>
+      </c>
+      <c r="B14">
+        <f>A14/1000</f>
+        <v>0.14826699999999998</v>
+      </c>
+      <c r="C14">
+        <f>1.3/2*1000</f>
+        <v>650</v>
+      </c>
+      <c r="D14">
+        <f>C14/B14</f>
+        <v>4383.9829496786206</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K2:K7">
@@ -17101,7 +17141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Layout complete and ready for manufacturing, still missing half of the output files which will be created next.
</commit_message>
<xml_diff>
--- a/DDR3 board timings.xlsx
+++ b/DDR3 board timings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16548" windowHeight="6036" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16548" windowHeight="6036" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Pin delays - All" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="1090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="1089">
   <si>
     <t>#Top: ios   Floorplan: io_1   Part: xc7z020clg484-1</t>
   </si>
@@ -3283,9 +3283,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>NEEDS UPDATE ON GB_* LINES</t>
   </si>
   <si>
     <t>ps/inch</t>
@@ -14227,8 +14224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14312,7 +14309,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D2">
-        <v>772.19399999999996</v>
+        <v>767.58100000000002</v>
       </c>
       <c r="F2">
         <v>24.315000000000001</v>
@@ -14322,7 +14319,7 @@
       </c>
       <c r="J2" s="5">
         <f>B2+(C2+H2)/1000*io_1!$J$1+(D2+F2*2+G2*2)/1000*io_1!$J$2</f>
-        <v>204.52178174599999</v>
+        <v>203.76089968700001</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="9" t="s">
@@ -14357,7 +14354,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D3">
-        <v>788.33699999999999</v>
+        <v>786.98599999999999</v>
       </c>
       <c r="F3">
         <v>24.315000000000001</v>
@@ -14367,7 +14364,7 @@
       </c>
       <c r="J3" s="5">
         <f>B3+(C3+H3)/1000*io_1!$J$1+(D3+F3*2+G3*2)/1000*io_1!$J$2</f>
-        <v>204.29395659500003</v>
+        <v>204.07111860200001</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -14381,14 +14378,14 @@
       </c>
       <c r="C4" s="11">
         <f>MAX(J2:J3)-MIN(J2:J3)</f>
-        <v>0.22782515099996203</v>
+        <v>0.3102189150000072</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>179</v>
       </c>
       <c r="J4" s="9">
         <f>AVERAGE(J2:J3)</f>
-        <v>204.40786917050002</v>
+        <v>203.91600914450001</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -14490,11 +14487,11 @@
       </c>
       <c r="K8" s="5">
         <f>$J$4-J8</f>
-        <v>-5.2119013004999601</v>
+        <v>-5.703761326499972</v>
       </c>
       <c r="L8" s="5">
         <f>K8/io_1!$J$2*1000</f>
-        <v>-31.598196349647818</v>
+        <v>-34.580196349647885</v>
       </c>
       <c r="M8" t="str">
         <f>IF(J8=$R$8, "Route","")</f>
@@ -14550,11 +14547,11 @@
       </c>
       <c r="K9" s="5">
         <f t="shared" ref="K9:K30" si="0">$J$4-J9</f>
-        <v>5.2212629994999986</v>
+        <v>4.7294029734999867</v>
       </c>
       <c r="L9" s="5">
         <f>K9/io_1!$J$2*1000</f>
-        <v>31.654953526369706</v>
+        <v>28.672953526369632</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" ref="M9:M30" si="1">IF(J9=$R$8, "Route","")</f>
@@ -14606,11 +14603,11 @@
       </c>
       <c r="K10" s="5">
         <f t="shared" si="0"/>
-        <v>-6.2709488544999772</v>
+        <v>-6.7628088804999891</v>
       </c>
       <c r="L10" s="5">
         <f>K10/io_1!$J$2*1000</f>
-        <v>-38.018884429772569</v>
+        <v>-41.00088442977264</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
@@ -14637,7 +14634,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D11">
-        <v>874.06399999999996</v>
+        <v>877.32600000000002</v>
       </c>
       <c r="F11">
         <v>9.0549999999999997</v>
@@ -14647,15 +14644,15 @@
       </c>
       <c r="J11" s="5">
         <f>B11+(C11+H11+E11)/1000*io_1!$J$1+(D11+F11*2+G11*2)/1000*io_1!$J$2</f>
-        <v>197.60096479600003</v>
+        <v>198.13900886200003</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="0"/>
-        <v>6.8069043744999931</v>
+        <v>5.7770002824999835</v>
       </c>
       <c r="L11" s="5">
         <f>K11/io_1!$J$2*1000</f>
-        <v>41.268222201002729</v>
+        <v>35.024222201002665</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="1"/>
@@ -14667,7 +14664,7 @@
       </c>
       <c r="S11">
         <f t="shared" si="3"/>
-        <v>197.60096479600003</v>
+        <v>198.13900886200003</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
@@ -14702,11 +14699,11 @@
       </c>
       <c r="K12" s="5">
         <f t="shared" si="0"/>
-        <v>4.1312060355000142</v>
+        <v>3.6393460095000023</v>
       </c>
       <c r="L12" s="5">
         <f>K12/io_1!$J$2*1000</f>
-        <v>25.046264682344894</v>
+        <v>22.064264682344824</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="1"/>
@@ -14747,11 +14744,11 @@
       </c>
       <c r="K13" s="5">
         <f t="shared" si="0"/>
-        <v>-0.19707006149999984</v>
+        <v>-0.68893008750001172</v>
       </c>
       <c r="L13" s="5">
         <f>K13/io_1!$J$2*1000</f>
-        <v>-1.1947767501500508</v>
+        <v>-4.1767767501501227</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="1"/>
@@ -14792,11 +14789,11 @@
       </c>
       <c r="K14" s="5">
         <f t="shared" si="0"/>
-        <v>7.5130887454999993</v>
+        <v>7.0212287194999874</v>
       </c>
       <c r="L14" s="5">
         <f>K14/io_1!$J$2*1000</f>
-        <v>45.549606503458762</v>
+        <v>42.567606503458691</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="1"/>
@@ -14823,7 +14820,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D15">
-        <v>860.48599999999999</v>
+        <v>845.89099999999996</v>
       </c>
       <c r="F15">
         <v>12.635</v>
@@ -14833,15 +14830,15 @@
       </c>
       <c r="J15" s="5">
         <f>B15+(C15+H15+E15)/1000*io_1!$J$1+(D15+F15*2+G15*2)/1000*io_1!$J$2</f>
-        <v>203.249860622</v>
+        <v>200.84251753699999</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="0"/>
-        <v>1.1580085485000211</v>
+        <v>3.0734916075000172</v>
       </c>
       <c r="L15" s="5">
         <f>K15/io_1!$J$2*1000</f>
-        <v>7.0206589458177735</v>
+        <v>18.633658945817746</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="1"/>
@@ -14853,7 +14850,7 @@
       </c>
       <c r="S15">
         <f t="shared" si="3"/>
-        <v>203.249860622</v>
+        <v>200.84251753699999</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
@@ -14882,11 +14879,11 @@
       </c>
       <c r="K16" s="5">
         <f t="shared" si="0"/>
-        <v>6.7056476635000308</v>
+        <v>6.2137876375000189</v>
       </c>
       <c r="L16" s="5">
         <f>K16/io_1!$J$2*1000</f>
-        <v>40.654333093856849</v>
+        <v>37.672333093856778</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="1"/>
@@ -14933,11 +14930,11 @@
       </c>
       <c r="K17" s="5">
         <f t="shared" si="0"/>
-        <v>0.12722212049999371</v>
+        <v>-0.36463790550001818</v>
       </c>
       <c r="L17" s="5">
         <f>K17/io_1!$J$2*1000</f>
-        <v>0.77130960695509176</v>
+        <v>-2.2106903930449802</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="1"/>
@@ -14978,11 +14975,11 @@
       </c>
       <c r="K18" s="5">
         <f t="shared" si="0"/>
-        <v>2.2357547585000361</v>
+        <v>1.7438947325000242</v>
       </c>
       <c r="L18" s="5">
         <f>K18/io_1!$J$2*1000</f>
-        <v>13.554711376051339</v>
+        <v>10.572711376051267</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="1"/>
@@ -15023,11 +15020,11 @@
       </c>
       <c r="K19" s="5">
         <f t="shared" si="0"/>
-        <v>8.0298281055000302</v>
+        <v>7.5379680795000183</v>
       </c>
       <c r="L19" s="5">
         <f>K19/io_1!$J$2*1000</f>
-        <v>48.682442452847532</v>
+        <v>45.700442452847454</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="1"/>
@@ -15068,11 +15065,11 @@
       </c>
       <c r="K20" s="5">
         <f t="shared" si="0"/>
-        <v>-2.1617687424999872</v>
+        <v>-2.6536287684999991</v>
       </c>
       <c r="L20" s="5">
         <f>K20/io_1!$J$2*1000</f>
-        <v>-13.106156323699624</v>
+        <v>-16.088156323699696</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="1"/>
@@ -15113,11 +15110,11 @@
       </c>
       <c r="K21" s="5">
         <f t="shared" si="0"/>
-        <v>5.4984093735000101</v>
+        <v>5.0065493474999982</v>
       </c>
       <c r="L21" s="5">
         <f>K21/io_1!$J$2*1000</f>
-        <v>33.335208972190451</v>
+        <v>30.35320897219038</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="1"/>
@@ -15158,11 +15155,11 @@
       </c>
       <c r="K22" s="5">
         <f t="shared" si="0"/>
-        <v>2.8151231705000157</v>
+        <v>2.3232631445000038</v>
       </c>
       <c r="L22" s="5">
         <f>K22/io_1!$J$2*1000</f>
-        <v>17.067248507060111</v>
+        <v>14.085248507060037</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="1"/>
@@ -15203,11 +15200,11 @@
       </c>
       <c r="K23" s="5">
         <f t="shared" si="0"/>
-        <v>8.0732258655000351</v>
+        <v>7.5813658395000232</v>
       </c>
       <c r="L23" s="5">
         <f>K23/io_1!$J$2*1000</f>
-        <v>48.945550071843208</v>
+        <v>45.963550071843137</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="1"/>
@@ -15248,11 +15245,11 @@
       </c>
       <c r="K24" s="5">
         <f t="shared" si="0"/>
-        <v>-0.66094212249996076</v>
+        <v>-1.1528021484999726</v>
       </c>
       <c r="L24" s="5">
         <f>K24/io_1!$J$2*1000</f>
-        <v>-4.0070941022047659</v>
+        <v>-6.9890941022048381</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="1"/>
@@ -15293,11 +15290,11 @@
       </c>
       <c r="K25" s="5">
         <f t="shared" si="0"/>
-        <v>-3.5653000964999819</v>
+        <v>-4.0571601224999938</v>
       </c>
       <c r="L25" s="5">
         <f>K25/io_1!$J$2*1000</f>
-        <v>-21.615346492424546</v>
+        <v>-24.597346492424617</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="1"/>
@@ -15338,11 +15335,11 @@
       </c>
       <c r="K26" s="5">
         <f t="shared" si="0"/>
-        <v>7.307619665499999</v>
+        <v>6.8157596394999871</v>
       </c>
       <c r="L26" s="5">
         <f>K26/io_1!$J$2*1000</f>
-        <v>44.303909020085719</v>
+        <v>41.321909020085648</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="1"/>
@@ -15383,11 +15380,11 @@
       </c>
       <c r="K27" s="5">
         <f t="shared" si="0"/>
-        <v>3.7454428584999846</v>
+        <v>3.2535828324999727</v>
       </c>
       <c r="L27" s="5">
         <f>K27/io_1!$J$2*1000</f>
-        <v>22.707498096311966</v>
+        <v>19.725498096311892</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="1"/>
@@ -15428,11 +15425,11 @@
       </c>
       <c r="K28" s="5">
         <f t="shared" si="0"/>
-        <v>-8.0211171215000263</v>
+        <v>-8.5129771475000382</v>
       </c>
       <c r="L28" s="5">
         <f>K28/io_1!$J$2*1000</f>
-        <v>-48.629630366247895</v>
+        <v>-51.611630366247958</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="1"/>
@@ -15473,11 +15470,11 @@
       </c>
       <c r="K29" s="5">
         <f t="shared" si="0"/>
-        <v>-2.0147760554999934</v>
+        <v>-2.5066360815000053</v>
       </c>
       <c r="L29" s="5">
         <f>K29/io_1!$J$2*1000</f>
-        <v>-12.214983694367104</v>
+        <v>-15.196983694367175</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="1"/>
@@ -15518,11 +15515,11 @@
       </c>
       <c r="K30" s="5">
         <f t="shared" si="0"/>
-        <v>-4.3890605499996127E-2</v>
+        <v>-0.53575063150000801</v>
       </c>
       <c r="L30" s="5">
         <f>K30/io_1!$J$2*1000</f>
-        <v>-0.26609559362929086</v>
+        <v>-3.2480955936293627</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="1"/>
@@ -15647,7 +15644,7 @@
       </c>
       <c r="O36" s="5">
         <f>MIN(J36:J46)</f>
-        <v>168.92994562700002</v>
+        <v>168.37755617400001</v>
       </c>
       <c r="Q36">
         <f>IF(D36=0,J36,0)</f>
@@ -15663,7 +15660,7 @@
       </c>
       <c r="T36">
         <f>MIN(S36:S46)</f>
-        <v>168.92994562700002</v>
+        <v>168.37755617400001</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
@@ -16004,7 +16001,7 @@
         <v>22.271000000000001</v>
       </c>
       <c r="D44">
-        <v>576.202</v>
+        <v>571.59</v>
       </c>
       <c r="F44">
         <v>24.315000000000001</v>
@@ -16014,15 +16011,15 @@
       </c>
       <c r="J44" s="5">
         <f>B44+(C44+H44+E44)/1000*io_1!$J$1+(D44+F44*2+G44*2)/1000*io_1!$J$2</f>
-        <v>169.13827329</v>
+        <v>168.37755617400001</v>
       </c>
       <c r="K44" s="5">
         <f t="shared" si="4"/>
-        <v>5.3792471490000082</v>
+        <v>6.1399642650000033</v>
       </c>
       <c r="L44" s="5">
         <f>K44/io_1!$J$2*1000</f>
-        <v>32.612764100325613</v>
+        <v>37.224764100325579</v>
       </c>
       <c r="M44" t="str">
         <f t="shared" si="5"/>
@@ -16034,7 +16031,7 @@
       </c>
       <c r="S44">
         <f t="shared" si="7"/>
-        <v>169.13827329</v>
+        <v>168.37755617400001</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
@@ -16133,7 +16130,7 @@
       </c>
       <c r="C47" s="9">
         <f>MAX(J36:J46)-MIN(J36:J46)</f>
-        <v>12.41914509099999</v>
+        <v>12.971534544000008</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>185</v>
@@ -16149,7 +16146,7 @@
       </c>
       <c r="C48" s="6">
         <f>T37-T36</f>
-        <v>12.41914509099999</v>
+        <v>12.971534544000008</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>186</v>
@@ -17088,16 +17085,16 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B13" t="s">
         <v>1087</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1088</v>
       </c>
       <c r="C13" t="s">
         <v>173</v>
       </c>
       <c r="D13" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -17663,10 +17660,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17674,7 +17671,7 @@
     <col min="1" max="1" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>157</v>
       </c>
@@ -17713,7 +17710,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1067</v>
       </c>
@@ -17739,7 +17736,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1069</v>
       </c>
@@ -17772,7 +17769,7 @@
       </c>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1070</v>
       </c>
@@ -17791,7 +17788,7 @@
       </c>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1068</v>
       </c>
@@ -17817,7 +17814,7 @@
         <v>39.808928713</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1071</v>
       </c>
@@ -17836,7 +17833,7 @@
       </c>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>1072</v>
       </c>
@@ -17862,7 +17859,7 @@
         <v>48.673219574999997</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>1073</v>
       </c>
@@ -17880,7 +17877,7 @@
         <v>69.773985947000014</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>1074</v>
       </c>
@@ -17906,12 +17903,12 @@
         <v>67.681123108500003</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>1078</v>
       </c>
       <c r="B11">
-        <v>1551.7239999999999</v>
+        <v>1558.643</v>
       </c>
       <c r="E11" s="14">
         <v>36.950000000000003</v>
@@ -17921,19 +17918,19 @@
       </c>
       <c r="K11" s="5">
         <f>(B11+I11+D11)/1000*io_1!$J$1+(C11+E11+F11+G11+H11)/1000*io_1!$J$2</f>
-        <v>249.74818043099998</v>
+        <v>250.77403980399998</v>
       </c>
       <c r="M11" s="8"/>
       <c r="O11" t="s">
         <v>1085</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="B12">
-        <v>1563.9280000000001</v>
+        <v>1570.846</v>
       </c>
       <c r="E12" s="14">
         <v>36.950000000000003</v>
@@ -17943,27 +17940,28 @@
       </c>
       <c r="K12" s="5">
         <f>(B12+I12+D12)/1000*io_1!$J$1+(C12+E12+F12+G12+H12)/1000*io_1!$J$2</f>
-        <v>248.99765287700001</v>
+        <v>250.02336398300002</v>
       </c>
       <c r="L12">
         <f>ABS(K11-K12)</f>
-        <v>0.75052755399997295</v>
+        <v>0.75067582099995889</v>
       </c>
       <c r="M12" s="15">
         <f>AVERAGE(K11:K12)</f>
-        <v>249.37291665399999</v>
+        <v>250.3987018935</v>
       </c>
       <c r="O12" s="5">
         <f>M3+M12</f>
-        <v>331.02456432450003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <v>332.05034956400004</v>
+      </c>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>1079</v>
       </c>
       <c r="B13">
-        <v>1801.173</v>
+        <v>1794.65</v>
       </c>
       <c r="E13" s="14">
         <v>36.950000000000003</v>
@@ -17973,16 +17971,16 @@
       </c>
       <c r="K13" s="5">
         <f>(B13+I13+D13)/1000*io_1!$J$1+(C13+E13+F13+G13+H13)/1000*io_1!$J$2</f>
-        <v>286.97505879099998</v>
+        <v>286.00791315000004</v>
       </c>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>1080</v>
       </c>
       <c r="B14">
-        <v>1803.741</v>
+        <v>1808.4659999999999</v>
       </c>
       <c r="E14" s="14">
         <v>36.950000000000003</v>
@@ -17992,30 +17990,30 @@
       </c>
       <c r="K14" s="5">
         <f>(B14+I14+D14)/1000*io_1!$J$1+(C14+E14+F14+G14+H14)/1000*io_1!$J$2</f>
-        <v>284.31218347100003</v>
+        <v>285.01274504599996</v>
       </c>
       <c r="L14">
         <f>ABS(K13-K14)</f>
-        <v>2.6628753199999551</v>
+        <v>0.99516810400007216</v>
       </c>
       <c r="M14" s="15">
         <f>AVERAGE(K13:K14)</f>
-        <v>285.64362113100003</v>
+        <v>285.510329098</v>
       </c>
       <c r="O14" s="5">
         <f>M5+M14</f>
-        <v>325.45254984400003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+        <v>325.319257811</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>1081</v>
       </c>
       <c r="B15">
-        <v>90.887</v>
+        <v>123.958</v>
       </c>
       <c r="C15">
-        <v>1564.1790000000001</v>
+        <v>1529.961</v>
       </c>
       <c r="E15" s="14">
         <v>27.895</v>
@@ -18028,19 +18026,19 @@
       </c>
       <c r="K15" s="5">
         <f>(B15+I15+D15)/1000*io_1!$J$1+(C15+E15+F15+G15+H15)/1000*io_1!$J$2</f>
-        <v>291.41306713</v>
+        <v>290.67238551300005</v>
       </c>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>1082</v>
       </c>
       <c r="B16">
-        <v>90.887</v>
+        <v>123.958</v>
       </c>
       <c r="C16">
-        <v>1576.954</v>
+        <v>1544.3579999999999</v>
       </c>
       <c r="E16" s="14">
         <v>27.895</v>
@@ -18053,19 +18051,19 @@
       </c>
       <c r="K16" s="5">
         <f>(B16+I16+D16)/1000*io_1!$J$1+(C16+E16+F16+G16+H16)/1000*io_1!$J$2</f>
-        <v>290.45998307500003</v>
+        <v>289.98683900399999</v>
       </c>
       <c r="L16">
         <f>ABS(K15-K16)</f>
-        <v>0.95308405499997662</v>
+        <v>0.68554650900006209</v>
       </c>
       <c r="M16" s="15">
         <f>AVERAGE(K15:K16)</f>
-        <v>290.93652510250001</v>
+        <v>290.32961225849999</v>
       </c>
       <c r="O16" s="5">
         <f>M7+M16</f>
-        <v>339.60974467750003</v>
+        <v>339.00283183350001</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -18097,10 +18095,10 @@
         <v>1084</v>
       </c>
       <c r="B18">
-        <v>90.887</v>
+        <v>123.958</v>
       </c>
       <c r="C18">
-        <v>1624.731</v>
+        <v>1591.6020000000001</v>
       </c>
       <c r="E18" s="14">
         <v>27.895</v>
@@ -18113,24 +18111,19 @@
       </c>
       <c r="K18" s="5">
         <f>(B18+I18+D18)/1000*io_1!$J$1+(C18+E18+F18+G18+H18)/1000*io_1!$J$2</f>
-        <v>298.34046478599998</v>
+        <v>297.77940609600006</v>
       </c>
       <c r="L18">
         <f>ABS(K17-K18)</f>
-        <v>0.8651694360000306</v>
+        <v>1.4262281259999554</v>
       </c>
       <c r="M18" s="15">
         <f>AVERAGE(K17:K18)</f>
-        <v>298.77304950400003</v>
+        <v>298.49252015900004</v>
       </c>
       <c r="O18" s="5">
         <f>M9+M18</f>
-        <v>366.45417261250003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>1086</v>
+        <v>366.17364326750004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start of work for RevB: Resolves #1: Symbol rotated and pairs swapped to facilitate routing. Minimal impact. Resolves #3: All pull-ups removed. Resolves #4: Series resistor added. Resolves #5: JTAG resistor placed on right line. Resolves #9: I2C pull-ups removed Resolves #13: ATCA LEDs no longer biased. Resolves #14: R109 removed.
</commit_message>
<xml_diff>
--- a/DDR3 board timings.xlsx
+++ b/DDR3 board timings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16548" windowHeight="6036" activeTab="5"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16548" windowHeight="6036" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pin delays - All" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="1093">
   <si>
     <t>#Top: ios   Floorplan: io_1   Part: xc7z020clg484-1</t>
   </si>
@@ -3292,6 +3292,18 @@
   </si>
   <si>
     <t>mil</t>
+  </si>
+  <si>
+    <t>Average data propagation:</t>
+  </si>
+  <si>
+    <t>Midrange of DQ and DM:</t>
+  </si>
+  <si>
+    <t>Midrange average with DDR clock:</t>
+  </si>
+  <si>
+    <t>Difference from DDR clock:</t>
   </si>
 </sst>
 </file>
@@ -4435,7 +4447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR405"/>
   <sheetViews>
-    <sheetView topLeftCell="A195" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G209" sqref="G209"/>
     </sheetView>
   </sheetViews>
@@ -12953,8 +12965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14222,10 +14234,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T64"/>
+  <dimension ref="A1:T65"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14403,9 +14415,6 @@
       <c r="L5" s="5"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G6">
-        <v>219.85499999999999</v>
-      </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -16139,6 +16148,13 @@
         <f>MAX(J41:J42)-MIN(J41:J42)</f>
         <v>0.36356349400000454</v>
       </c>
+      <c r="H47" s="6" t="s">
+        <v>1090</v>
+      </c>
+      <c r="J47" s="5">
+        <f>(MAX(J36:J40,J43:J46)+MIN(J36:J40,J43:J46))/2</f>
+        <v>174.86332344600001</v>
+      </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B48" s="6" t="s">
@@ -16155,6 +16171,30 @@
         <f>AVERAGE(J41:J42)</f>
         <v>174.51752043900001</v>
       </c>
+      <c r="H48" s="6" t="s">
+        <v>1089</v>
+      </c>
+      <c r="J48" s="5">
+        <f>AVERAGE(J36:J40,J43:J46)</f>
+        <v>172.59774147344444</v>
+      </c>
+      <c r="K48" s="5"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="E49" s="6" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F49" s="5">
+        <f>$J$4-F48</f>
+        <v>29.3984887055</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>1091</v>
+      </c>
+      <c r="K49" s="5">
+        <f>AVERAGE(J47,$J$4)</f>
+        <v>189.38966629525001</v>
+      </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
@@ -16737,6 +16777,13 @@
         <f>MAX(J57:J58)-MIN(J57:J58)</f>
         <v>0.30773881800001845</v>
       </c>
+      <c r="H63" s="6" t="s">
+        <v>1090</v>
+      </c>
+      <c r="J63" s="5">
+        <f>(MAX(J52:J56,J59:J62)+MIN(J52:J56,J59:J62))/2</f>
+        <v>156.7526166175</v>
+      </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B64" s="6" t="s">
@@ -16752,6 +16799,30 @@
       <c r="F64" s="5">
         <f>AVERAGE(J57:J58)</f>
         <v>157.41322902900001</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>1089</v>
+      </c>
+      <c r="J64" s="5">
+        <f>AVERAGE(J52:J56,J59:J62)</f>
+        <v>155.24309455600002</v>
+      </c>
+      <c r="K64" s="5"/>
+    </row>
+    <row r="65" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E65" s="6" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F65" s="5">
+        <f>$J$4-F64</f>
+        <v>46.502780115500002</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>1091</v>
+      </c>
+      <c r="K65" s="5">
+        <f>AVERAGE(J63,$J$4)</f>
+        <v>180.33431288100002</v>
       </c>
     </row>
   </sheetData>
@@ -17662,7 +17733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>